<commit_message>
Add new table format with the enrollment variables
</commit_message>
<xml_diff>
--- a/03_Tables/muestra_1porciento/SelfUpdate_twfe_wage_heterogeneity.xlsx
+++ b/03_Tables/muestra_1porciento/SelfUpdate_twfe_wage_heterogeneity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcomedina/ITAM Seira Research Dropbox/Marco Alejandro Medina/imss_rpci/03_Tables/muestra_1porciento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967A2D27-5DA5-CC46-A699-3E4BE8EFD41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE84956-5C06-A84B-9F71-6DCB09422BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{5F2EF16D-A70A-3F40-9EFD-AA737EECFF16}"/>
   </bookViews>
@@ -274,7 +274,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +339,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -368,40 +371,40 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3" t="str">
-            <v>12.7***</v>
+            <v>9.3***</v>
           </cell>
           <cell r="C3">
-            <v>1</v>
+            <v>-2.8</v>
           </cell>
           <cell r="D3">
-            <v>2</v>
+            <v>-1.7</v>
           </cell>
           <cell r="E3" t="str">
-            <v>12.4**</v>
+            <v>10.5**</v>
           </cell>
           <cell r="F3">
-            <v>4.7</v>
+            <v>1.6</v>
           </cell>
           <cell r="G3" t="str">
-            <v>20.9**</v>
+            <v>18.5**</v>
           </cell>
           <cell r="H3">
-            <v>5.8</v>
+            <v>2.9</v>
           </cell>
           <cell r="I3">
-            <v>9.4</v>
+            <v>6.6</v>
           </cell>
           <cell r="J3">
-            <v>7.2</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>7.7*</v>
+            <v>2.1</v>
+          </cell>
+          <cell r="K3">
+            <v>5.7</v>
           </cell>
           <cell r="L3">
-            <v>3.2</v>
+            <v>-0.2</v>
           </cell>
           <cell r="M3" t="str">
-            <v>8.8**</v>
+            <v>8.1**</v>
           </cell>
         </row>
         <row r="4">
@@ -409,37 +412,37 @@
             <v>2.96</v>
           </cell>
           <cell r="C4">
-            <v>2.71</v>
+            <v>2.72</v>
           </cell>
           <cell r="D4">
-            <v>4.26</v>
+            <v>4.2300000000000004</v>
           </cell>
           <cell r="E4">
             <v>5.26</v>
           </cell>
           <cell r="F4">
-            <v>4.1900000000000004</v>
+            <v>4.22</v>
           </cell>
           <cell r="G4">
-            <v>9.06</v>
+            <v>9.1300000000000008</v>
           </cell>
           <cell r="H4">
             <v>4.0599999999999996</v>
           </cell>
           <cell r="I4">
-            <v>7.69</v>
+            <v>7.81</v>
           </cell>
           <cell r="J4">
             <v>4.72</v>
           </cell>
           <cell r="K4">
-            <v>4.03</v>
+            <v>4</v>
           </cell>
           <cell r="L4">
-            <v>2.2799999999999998</v>
+            <v>2.2599999999999998</v>
           </cell>
           <cell r="M4">
-            <v>4.09</v>
+            <v>4.05</v>
           </cell>
         </row>
         <row r="5">
@@ -465,16 +468,16 @@
             <v>387.1***</v>
           </cell>
           <cell r="I5" t="str">
-            <v>478.6***</v>
+            <v>478.7***</v>
           </cell>
           <cell r="J5" t="str">
-            <v>456.1***</v>
+            <v>456.2***</v>
           </cell>
           <cell r="K5" t="str">
-            <v>575.4***</v>
+            <v>575.5***</v>
           </cell>
           <cell r="L5" t="str">
-            <v>360.7***</v>
+            <v>360.8***</v>
           </cell>
           <cell r="M5" t="str">
             <v>567.8***</v>
@@ -532,28 +535,28 @@
             <v>834197</v>
           </cell>
           <cell r="F7">
-            <v>1638601</v>
+            <v>1638574</v>
           </cell>
           <cell r="G7">
-            <v>443291</v>
+            <v>443213</v>
           </cell>
           <cell r="H7">
-            <v>1200875</v>
+            <v>1200886</v>
           </cell>
           <cell r="I7">
-            <v>353164</v>
+            <v>353227</v>
           </cell>
           <cell r="J7">
-            <v>1342614</v>
+            <v>1342575</v>
           </cell>
           <cell r="K7">
-            <v>663882</v>
+            <v>663920</v>
           </cell>
           <cell r="L7">
-            <v>3000417</v>
+            <v>3000398</v>
           </cell>
           <cell r="M7">
-            <v>1566956</v>
+            <v>1567062</v>
           </cell>
         </row>
         <row r="8">
@@ -573,19 +576,19 @@
             <v>463.7</v>
           </cell>
           <cell r="G8">
-            <v>317.5</v>
+            <v>317.60000000000002</v>
           </cell>
           <cell r="H8">
             <v>387.2</v>
           </cell>
           <cell r="I8">
-            <v>478.7</v>
+            <v>478.8</v>
           </cell>
           <cell r="J8">
             <v>456.2</v>
           </cell>
           <cell r="K8">
-            <v>575.6</v>
+            <v>575.5</v>
           </cell>
           <cell r="L8">
             <v>360.8</v>
@@ -611,63 +614,63 @@
             <v>65310</v>
           </cell>
           <cell r="G9">
-            <v>24002</v>
+            <v>23999</v>
           </cell>
           <cell r="H9">
-            <v>49401</v>
+            <v>49402</v>
           </cell>
           <cell r="I9">
-            <v>14143</v>
+            <v>14145</v>
           </cell>
           <cell r="J9">
-            <v>58131</v>
+            <v>58129</v>
           </cell>
           <cell r="K9">
-            <v>24306</v>
+            <v>24307</v>
           </cell>
           <cell r="L9">
-            <v>158754</v>
+            <v>158757</v>
           </cell>
           <cell r="M9">
-            <v>62049</v>
+            <v>62052</v>
           </cell>
         </row>
         <row r="10">
           <cell r="B10">
-            <v>109938</v>
+            <v>109939</v>
           </cell>
           <cell r="C10">
             <v>64446</v>
           </cell>
           <cell r="D10">
-            <v>36039</v>
+            <v>36040</v>
           </cell>
           <cell r="E10">
-            <v>36669</v>
+            <v>36671</v>
           </cell>
           <cell r="F10">
-            <v>35787</v>
+            <v>35790</v>
           </cell>
           <cell r="G10">
-            <v>31310</v>
+            <v>31301</v>
           </cell>
           <cell r="H10">
-            <v>39397</v>
+            <v>39408</v>
           </cell>
           <cell r="I10">
-            <v>13749</v>
+            <v>13750</v>
           </cell>
           <cell r="J10">
-            <v>50968</v>
+            <v>50965</v>
           </cell>
           <cell r="K10">
-            <v>10109</v>
+            <v>10108</v>
           </cell>
           <cell r="L10">
-            <v>137679</v>
+            <v>137682</v>
           </cell>
           <cell r="M10">
-            <v>18849</v>
+            <v>18855</v>
           </cell>
         </row>
       </sheetData>
@@ -686,40 +689,40 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3" t="str">
-            <v>0.03***</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>0.01**</v>
+            <v>0.02***</v>
+          </cell>
+          <cell r="C3">
+            <v>0</v>
           </cell>
           <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>0.03**</v>
+          </cell>
+          <cell r="F3">
             <v>0.01</v>
           </cell>
-          <cell r="E3" t="str">
-            <v>0.03***</v>
-          </cell>
-          <cell r="F3" t="str">
-            <v>0.01*</v>
-          </cell>
           <cell r="G3" t="str">
-            <v>0.04**</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>0.02*</v>
-          </cell>
-          <cell r="I3" t="str">
-            <v>0.03*</v>
+            <v>0.03**</v>
+          </cell>
+          <cell r="H3">
+            <v>0.01</v>
+          </cell>
+          <cell r="I3">
+            <v>0.02</v>
           </cell>
           <cell r="J3" t="str">
-            <v>0.03***</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>0.01**</v>
-          </cell>
-          <cell r="L3" t="str">
-            <v>0.01***</v>
+            <v>0.02**</v>
+          </cell>
+          <cell r="K3">
+            <v>0.01</v>
+          </cell>
+          <cell r="L3">
+            <v>0.01</v>
           </cell>
           <cell r="M3" t="str">
-            <v>0.02***</v>
+            <v>0.02**</v>
           </cell>
         </row>
         <row r="4">
@@ -745,7 +748,7 @@
             <v>8.0000000000000002E-3</v>
           </cell>
           <cell r="I4">
-            <v>1.4E-2</v>
+            <v>1.4999999999999999E-2</v>
           </cell>
           <cell r="J4">
             <v>8.0000000000000002E-3</v>
@@ -890,68 +893,68 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3">
-            <v>9.4</v>
+            <v>-1.1000000000000001</v>
           </cell>
           <cell r="C3" t="str">
-            <v>16.3*</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>7.8**</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>8.2*</v>
-          </cell>
-          <cell r="F3" t="str">
-            <v>12.3*</v>
+            <v>14.0*</v>
+          </cell>
+          <cell r="D3">
+            <v>3.3</v>
+          </cell>
+          <cell r="E3">
+            <v>3.7</v>
+          </cell>
+          <cell r="F3">
+            <v>6.7</v>
           </cell>
           <cell r="G3">
-            <v>-6.2</v>
+            <v>-8.6</v>
           </cell>
           <cell r="H3" t="str">
-            <v>8.8**</v>
+            <v>8.1**</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>16.23</v>
+            <v>12.05</v>
           </cell>
           <cell r="C4">
-            <v>8.43</v>
+            <v>8.34</v>
           </cell>
           <cell r="D4">
-            <v>3.8</v>
+            <v>3.81</v>
           </cell>
           <cell r="E4">
-            <v>4.6399999999999997</v>
+            <v>4.63</v>
           </cell>
           <cell r="F4">
-            <v>6.56</v>
+            <v>6.64</v>
           </cell>
           <cell r="G4">
-            <v>6.27</v>
+            <v>6.32</v>
           </cell>
           <cell r="H4">
-            <v>4.09</v>
+            <v>4.05</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>221.9***</v>
+            <v>221.7***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>234.2***</v>
+            <v>234.3***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>327.2***</v>
+            <v>327.3***</v>
           </cell>
           <cell r="E5" t="str">
-            <v>436.7***</v>
+            <v>436.8***</v>
           </cell>
           <cell r="F5" t="str">
-            <v>495.0***</v>
+            <v>494.9***</v>
           </cell>
           <cell r="G5" t="str">
-            <v>502.9***</v>
+            <v>503.0***</v>
           </cell>
           <cell r="H5" t="str">
             <v>567.8***</v>
@@ -959,7 +962,7 @@
         </row>
         <row r="6">
           <cell r="B6">
-            <v>0.11</v>
+            <v>0.08</v>
           </cell>
           <cell r="C6">
             <v>0.08</v>
@@ -982,30 +985,30 @@
         </row>
         <row r="7">
           <cell r="B7">
-            <v>75072</v>
+            <v>75017</v>
           </cell>
           <cell r="C7">
-            <v>327278</v>
+            <v>327260</v>
           </cell>
           <cell r="D7">
-            <v>1229857</v>
+            <v>1230059</v>
           </cell>
           <cell r="E7">
-            <v>1379195</v>
+            <v>1378921</v>
           </cell>
           <cell r="F7">
-            <v>685360</v>
+            <v>685465</v>
           </cell>
           <cell r="G7">
-            <v>647223</v>
+            <v>647157</v>
           </cell>
           <cell r="H7">
-            <v>1566956</v>
+            <v>1567062</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8">
-            <v>222</v>
+            <v>221.7</v>
           </cell>
           <cell r="C8">
             <v>234.4</v>
@@ -1014,10 +1017,10 @@
             <v>327.3</v>
           </cell>
           <cell r="E8">
-            <v>436.8</v>
+            <v>436.9</v>
           </cell>
           <cell r="F8">
-            <v>495.1</v>
+            <v>495</v>
           </cell>
           <cell r="G8">
             <v>502.9</v>
@@ -1028,48 +1031,48 @@
         </row>
         <row r="9">
           <cell r="B9">
-            <v>3214</v>
+            <v>3212</v>
           </cell>
           <cell r="C9">
-            <v>14491</v>
+            <v>14490</v>
           </cell>
           <cell r="D9">
-            <v>54228</v>
+            <v>54234</v>
           </cell>
           <cell r="E9">
-            <v>59133</v>
+            <v>59122</v>
           </cell>
           <cell r="F9">
-            <v>28758</v>
+            <v>28764</v>
           </cell>
           <cell r="G9">
-            <v>26815</v>
+            <v>26814</v>
           </cell>
           <cell r="H9">
-            <v>62049</v>
+            <v>62052</v>
           </cell>
         </row>
         <row r="10">
           <cell r="B10">
-            <v>4158</v>
+            <v>4154</v>
           </cell>
           <cell r="C10">
-            <v>20517</v>
+            <v>20516</v>
           </cell>
           <cell r="D10">
-            <v>72914</v>
+            <v>72915</v>
           </cell>
           <cell r="E10">
-            <v>53372</v>
+            <v>53354</v>
           </cell>
           <cell r="F10">
-            <v>21616</v>
+            <v>21623</v>
           </cell>
           <cell r="G10">
-            <v>15879</v>
+            <v>15878</v>
           </cell>
           <cell r="H10">
-            <v>18849</v>
+            <v>18855</v>
           </cell>
         </row>
       </sheetData>
@@ -1088,30 +1091,30 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3">
-            <v>0.04</v>
+            <v>0.01</v>
           </cell>
           <cell r="C3" t="str">
-            <v>0.04**</v>
+            <v>0.03**</v>
           </cell>
           <cell r="D3" t="str">
-            <v>0.02***</v>
+            <v>0.01*</v>
           </cell>
           <cell r="E3" t="str">
-            <v>0.03***</v>
+            <v>0.02**</v>
           </cell>
           <cell r="F3" t="str">
-            <v>0.03***</v>
+            <v>0.02*</v>
           </cell>
           <cell r="G3">
             <v>-0.01</v>
           </cell>
           <cell r="H3" t="str">
-            <v>0.02***</v>
+            <v>0.02**</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>4.2999999999999997E-2</v>
+            <v>3.1E-2</v>
           </cell>
           <cell r="C4">
             <v>1.4999999999999999E-2</v>
@@ -1507,7 +1510,7 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F19"/>
+      <selection activeCell="F19" sqref="B3:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,16 +1573,16 @@
       </c>
       <c r="C6" s="5" t="str" cm="1">
         <f t="array" ref="C6:F9">[1]twfe_sal_cierre_heterogeneity!$B$3:$E$6</f>
-        <v>12.7***</v>
+        <v>9.3***</v>
       </c>
       <c r="D6" s="17">
-        <v>1</v>
+        <v>-2.8</v>
       </c>
       <c r="E6" s="17">
-        <v>2</v>
+        <v>-1.7</v>
       </c>
       <c r="F6" s="5" t="str">
-        <v>12.4**</v>
+        <v>10.5**</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -1590,10 +1593,10 @@
         <v>2.96</v>
       </c>
       <c r="D7" s="11">
-        <v>2.71</v>
+        <v>2.72</v>
       </c>
       <c r="E7" s="11">
-        <v>4.26</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="F7" s="11">
         <v>5.26</v>
@@ -1666,16 +1669,16 @@
       </c>
       <c r="C12" s="5" t="str" cm="1">
         <f t="array" ref="C12:F15">[2]twfe_log_sal_cierre_heterogenei!$B$3:$E$6</f>
-        <v>0.03***</v>
-      </c>
-      <c r="D12" s="5" t="str">
-        <v>0.01**</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.01</v>
+        <v>0.02***</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0</v>
       </c>
       <c r="F12" s="5" t="str">
-        <v>0.03***</v>
+        <v>0.03**</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
@@ -1789,16 +1792,16 @@
         <v>19</v>
       </c>
       <c r="C19" s="9">
-        <v>109938</v>
+        <v>109939</v>
       </c>
       <c r="D19" s="9">
         <v>64446</v>
       </c>
       <c r="E19" s="9">
-        <v>36039</v>
+        <v>36040</v>
       </c>
       <c r="F19" s="9">
-        <v>36669</v>
+        <v>36671</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1924,28 +1927,28 @@
       </c>
       <c r="C6" s="5" cm="1">
         <f t="array" ref="C6:J9">[1]twfe_sal_cierre_heterogeneity!$F$3:$M$6</f>
-        <v>4.7</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="5" t="str">
-        <v>20.9**</v>
+        <v>18.5**</v>
       </c>
       <c r="E6" s="5">
-        <v>5.8</v>
+        <v>2.9</v>
       </c>
       <c r="F6" s="5">
-        <v>9.4</v>
+        <v>6.6</v>
       </c>
       <c r="G6" s="5">
-        <v>7.2</v>
-      </c>
-      <c r="H6" s="5" t="str">
-        <v>7.7*</v>
+        <v>2.1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.7</v>
       </c>
       <c r="I6" s="5">
-        <v>3.2</v>
+        <v>-0.2</v>
       </c>
       <c r="J6" s="5" t="str">
-        <v>8.8**</v>
+        <v>8.1**</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
@@ -1953,28 +1956,28 @@
         <v>0</v>
       </c>
       <c r="C7" s="11">
-        <v>4.1900000000000004</v>
+        <v>4.22</v>
       </c>
       <c r="D7" s="11">
-        <v>9.06</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="E7" s="11">
         <v>4.0599999999999996</v>
       </c>
       <c r="F7" s="11">
-        <v>7.69</v>
+        <v>7.81</v>
       </c>
       <c r="G7" s="11">
         <v>4.72</v>
       </c>
       <c r="H7" s="11">
-        <v>4.03</v>
+        <v>4</v>
       </c>
       <c r="I7" s="11">
-        <v>2.2799999999999998</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J7" s="11">
-        <v>4.09</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -1991,16 +1994,16 @@
         <v>387.1***</v>
       </c>
       <c r="F8" s="5" t="str">
-        <v>478.6***</v>
+        <v>478.7***</v>
       </c>
       <c r="G8" s="5" t="str">
-        <v>456.1***</v>
+        <v>456.2***</v>
       </c>
       <c r="H8" s="5" t="str">
-        <v>575.4***</v>
+        <v>575.5***</v>
       </c>
       <c r="I8" s="5" t="str">
-        <v>360.7***</v>
+        <v>360.8***</v>
       </c>
       <c r="J8" s="5" t="str">
         <v>567.8***</v>
@@ -2044,19 +2047,19 @@
         <v>463.7</v>
       </c>
       <c r="D10" s="5">
-        <v>317.5</v>
+        <v>317.60000000000002</v>
       </c>
       <c r="E10" s="5">
         <v>387.2</v>
       </c>
       <c r="F10" s="5">
-        <v>478.7</v>
+        <v>478.8</v>
       </c>
       <c r="G10" s="5">
         <v>456.2</v>
       </c>
       <c r="H10" s="5">
-        <v>575.6</v>
+        <v>575.5</v>
       </c>
       <c r="I10" s="5">
         <v>360.8</v>
@@ -2084,30 +2087,30 @@
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="14" t="str" cm="1">
+      <c r="C12" s="14" cm="1">
         <f t="array" ref="C12:J15">[2]twfe_log_sal_cierre_heterogenei!$F$3:$M$6</f>
-        <v>0.01*</v>
+        <v>0.01</v>
       </c>
       <c r="D12" s="14" t="str">
-        <v>0.04**</v>
-      </c>
-      <c r="E12" s="14" t="str">
-        <v>0.02*</v>
-      </c>
-      <c r="F12" s="14" t="str">
-        <v>0.03*</v>
+        <v>0.03**</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.02</v>
       </c>
       <c r="G12" s="14" t="str">
-        <v>0.03***</v>
-      </c>
-      <c r="H12" s="14" t="str">
-        <v>0.01**</v>
-      </c>
-      <c r="I12" s="14" t="str">
-        <v>0.01***</v>
+        <v>0.02**</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.01</v>
       </c>
       <c r="J12" s="14" t="str">
-        <v>0.02***</v>
+        <v>0.02**</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -2124,7 +2127,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F13" s="11">
-        <v>1.4E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G13" s="11">
         <v>8.0000000000000002E-3</v>
@@ -2233,28 +2236,28 @@
       </c>
       <c r="C17" s="10" cm="1">
         <f t="array" ref="C17:J17">[1]twfe_sal_cierre_heterogeneity!$F$7:$M$7</f>
-        <v>1638601</v>
+        <v>1638574</v>
       </c>
       <c r="D17" s="10">
-        <v>443291</v>
+        <v>443213</v>
       </c>
       <c r="E17" s="10">
-        <v>1200875</v>
+        <v>1200886</v>
       </c>
       <c r="F17" s="10">
-        <v>353164</v>
+        <v>353227</v>
       </c>
       <c r="G17" s="10">
-        <v>1342614</v>
+        <v>1342575</v>
       </c>
       <c r="H17" s="10">
-        <v>663882</v>
+        <v>663920</v>
       </c>
       <c r="I17" s="10">
-        <v>3000417</v>
+        <v>3000398</v>
       </c>
       <c r="J17" s="10">
-        <v>1566956</v>
+        <v>1567062</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -2266,25 +2269,25 @@
         <v>65310</v>
       </c>
       <c r="D18" s="13">
-        <v>24002</v>
+        <v>23999</v>
       </c>
       <c r="E18" s="13">
-        <v>49401</v>
+        <v>49402</v>
       </c>
       <c r="F18" s="13">
-        <v>14143</v>
+        <v>14145</v>
       </c>
       <c r="G18" s="13">
-        <v>58131</v>
+        <v>58129</v>
       </c>
       <c r="H18" s="13">
-        <v>24306</v>
+        <v>24307</v>
       </c>
       <c r="I18" s="13">
-        <v>158754</v>
+        <v>158757</v>
       </c>
       <c r="J18" s="13">
-        <v>62049</v>
+        <v>62052</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2292,28 +2295,28 @@
         <v>19</v>
       </c>
       <c r="C19" s="9">
-        <v>35787</v>
+        <v>35790</v>
       </c>
       <c r="D19" s="9">
-        <v>31310</v>
+        <v>31301</v>
       </c>
       <c r="E19" s="9">
-        <v>39397</v>
+        <v>39408</v>
       </c>
       <c r="F19" s="9">
-        <v>13749</v>
+        <v>13750</v>
       </c>
       <c r="G19" s="9">
-        <v>50968</v>
+        <v>50965</v>
       </c>
       <c r="H19" s="9">
-        <v>10109</v>
+        <v>10108</v>
       </c>
       <c r="I19" s="9">
-        <v>137679</v>
+        <v>137682</v>
       </c>
       <c r="J19" s="9">
-        <v>18849</v>
+        <v>18855</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -2341,7 +2344,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="B3" sqref="B3:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2437,25 +2440,25 @@
       </c>
       <c r="C6" s="5" cm="1">
         <f t="array" ref="C6:I9">[3]twfe_sal_cierre_heterogeneity_f!$B$3:$H$6</f>
-        <v>9.4</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="D6" s="5" t="str">
-        <v>16.3*</v>
-      </c>
-      <c r="E6" s="5" t="str">
-        <v>7.8**</v>
-      </c>
-      <c r="F6" s="5" t="str">
-        <v>8.2*</v>
-      </c>
-      <c r="G6" s="5" t="str">
-        <v>12.3*</v>
+        <v>14.0*</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="G6" s="5">
+        <v>6.7</v>
       </c>
       <c r="H6" s="5">
-        <v>-6.2</v>
+        <v>-8.6</v>
       </c>
       <c r="I6" s="5" t="str">
-        <v>8.8**</v>
+        <v>8.1**</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -2465,25 +2468,25 @@
         <v>0</v>
       </c>
       <c r="C7" s="19">
-        <v>16.23</v>
+        <v>12.05</v>
       </c>
       <c r="D7" s="19">
-        <v>8.43</v>
+        <v>8.34</v>
       </c>
       <c r="E7" s="19">
-        <v>3.8</v>
+        <v>3.81</v>
       </c>
       <c r="F7" s="19">
-        <v>4.6399999999999997</v>
+        <v>4.63</v>
       </c>
       <c r="G7" s="19">
-        <v>6.56</v>
+        <v>6.64</v>
       </c>
       <c r="H7" s="19">
-        <v>6.27</v>
+        <v>6.32</v>
       </c>
       <c r="I7" s="19">
-        <v>4.09</v>
+        <v>4.05</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -2493,22 +2496,22 @@
         <v>12</v>
       </c>
       <c r="C8" s="5" t="str">
-        <v>221.9***</v>
+        <v>221.7***</v>
       </c>
       <c r="D8" s="5" t="str">
-        <v>234.2***</v>
+        <v>234.3***</v>
       </c>
       <c r="E8" s="5" t="str">
-        <v>327.2***</v>
+        <v>327.3***</v>
       </c>
       <c r="F8" s="5" t="str">
-        <v>436.7***</v>
+        <v>436.8***</v>
       </c>
       <c r="G8" s="5" t="str">
-        <v>495.0***</v>
+        <v>494.9***</v>
       </c>
       <c r="H8" s="5" t="str">
-        <v>502.9***</v>
+        <v>503.0***</v>
       </c>
       <c r="I8" s="5" t="str">
         <v>567.8***</v>
@@ -2519,7 +2522,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="19">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="D9" s="19">
         <v>0.08</v>
@@ -2548,7 +2551,7 @@
       </c>
       <c r="C10" s="20" cm="1">
         <f t="array" ref="C10:I10">[3]twfe_sal_cierre_heterogeneity_f!$B$8:$H$8</f>
-        <v>222</v>
+        <v>221.7</v>
       </c>
       <c r="D10" s="20">
         <v>234.4</v>
@@ -2557,10 +2560,10 @@
         <v>327.3</v>
       </c>
       <c r="F10" s="20">
-        <v>436.8</v>
+        <v>436.9</v>
       </c>
       <c r="G10" s="20">
-        <v>495.1</v>
+        <v>495</v>
       </c>
       <c r="H10" s="20">
         <v>502.9</v>
@@ -2593,25 +2596,25 @@
       </c>
       <c r="C12" s="5" cm="1">
         <f t="array" ref="C12:I15">[4]twfe_log_sal_cierre_heterogenei!$B$3:$H$6</f>
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="D12" s="5" t="str">
-        <v>0.04**</v>
+        <v>0.03**</v>
       </c>
       <c r="E12" s="5" t="str">
-        <v>0.02***</v>
+        <v>0.01*</v>
       </c>
       <c r="F12" s="5" t="str">
-        <v>0.03***</v>
+        <v>0.02**</v>
       </c>
       <c r="G12" s="5" t="str">
-        <v>0.03***</v>
+        <v>0.02*</v>
       </c>
       <c r="H12" s="5">
         <v>-0.01</v>
       </c>
       <c r="I12" s="5" t="str">
-        <v>0.02***</v>
+        <v>0.02**</v>
       </c>
       <c r="J12" s="4"/>
     </row>
@@ -2621,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="11">
-        <v>4.2999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D13" s="11">
         <v>1.4999999999999999E-2</v>
@@ -2733,25 +2736,25 @@
       </c>
       <c r="C17" s="12" cm="1">
         <f t="array" ref="C17:I17">[3]twfe_sal_cierre_heterogeneity_f!$B$7:$H$7</f>
-        <v>75072</v>
+        <v>75017</v>
       </c>
       <c r="D17" s="12">
-        <v>327278</v>
+        <v>327260</v>
       </c>
       <c r="E17" s="12">
-        <v>1229857</v>
+        <v>1230059</v>
       </c>
       <c r="F17" s="12">
-        <v>1379195</v>
+        <v>1378921</v>
       </c>
       <c r="G17" s="12">
-        <v>685360</v>
+        <v>685465</v>
       </c>
       <c r="H17" s="12">
-        <v>647223</v>
+        <v>647157</v>
       </c>
       <c r="I17" s="12">
-        <v>1566956</v>
+        <v>1567062</v>
       </c>
       <c r="J17" s="4"/>
     </row>
@@ -2762,25 +2765,25 @@
       </c>
       <c r="C18" s="12" cm="1">
         <f t="array" ref="C18:I19">[3]twfe_sal_cierre_heterogeneity_f!$B$9:$H$10</f>
-        <v>3214</v>
+        <v>3212</v>
       </c>
       <c r="D18" s="13">
-        <v>14491</v>
+        <v>14490</v>
       </c>
       <c r="E18" s="13">
-        <v>54228</v>
+        <v>54234</v>
       </c>
       <c r="F18" s="13">
-        <v>59133</v>
+        <v>59122</v>
       </c>
       <c r="G18" s="13">
-        <v>28758</v>
+        <v>28764</v>
       </c>
       <c r="H18" s="13">
-        <v>26815</v>
+        <v>26814</v>
       </c>
       <c r="I18" s="13">
-        <v>62049</v>
+        <v>62052</v>
       </c>
       <c r="J18" s="4"/>
     </row>
@@ -2790,25 +2793,25 @@
         <v>19</v>
       </c>
       <c r="C19" s="9">
-        <v>4158</v>
+        <v>4154</v>
       </c>
       <c r="D19" s="9">
-        <v>20517</v>
+        <v>20516</v>
       </c>
       <c r="E19" s="9">
-        <v>72914</v>
+        <v>72915</v>
       </c>
       <c r="F19" s="9">
-        <v>53372</v>
+        <v>53354</v>
       </c>
       <c r="G19" s="9">
-        <v>21616</v>
+        <v>21623</v>
       </c>
       <c r="H19" s="9">
-        <v>15879</v>
+        <v>15878</v>
       </c>
       <c r="I19" s="9">
-        <v>18849</v>
+        <v>18855</v>
       </c>
       <c r="J19" s="4"/>
     </row>

</xml_diff>